<commit_message>
Added Digikey BOM V2
</commit_message>
<xml_diff>
--- a/BOMs/Plane_Project_Kicad_BOM_V2.xlsx
+++ b/BOMs/Plane_Project_Kicad_BOM_V2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>0.1uF</t>
   </si>
@@ -239,7 +239,10 @@
     <t>MCP601-xP Socket</t>
   </si>
   <si>
-    <t>Order Quantity</t>
+    <t>Min Order Quantity</t>
+  </si>
+  <si>
+    <t>Quantity Ordered</t>
   </si>
 </sst>
 </file>
@@ -311,7 +314,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -587,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,11 +613,12 @@
     <col min="2" max="2" width="88.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="17.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -619,8 +634,11 @@
       <c r="E1" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -637,8 +655,11 @@
         <f>MAX(0, C2-D2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -656,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -674,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -691,8 +712,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -709,8 +733,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -728,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -746,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -763,8 +790,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -781,8 +811,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -818,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -836,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -853,8 +886,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -871,8 +907,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -890,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -908,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -925,8 +964,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -944,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -962,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -980,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -998,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1034,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1052,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -1088,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -1105,8 +1147,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1124,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1141,8 +1186,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -1160,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
@@ -1178,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1196,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -1214,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1250,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
@@ -1268,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -1286,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -1304,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -1321,8 +1369,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>30</v>
       </c>
@@ -1344,6 +1395,11 @@
   <sortState ref="A2:C74">
     <sortCondition ref="A2:A74"/>
   </sortState>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>